<commit_message>
Remove any reference to L-BFGS-B algorithm
</commit_message>
<xml_diff>
--- a/examples/2_circle2circle_analysis_files/circle-to-same-circle_deltaV.xlsx
+++ b/examples/2_circle2circle_analysis_files/circle-to-same-circle_deltaV.xlsx
@@ -8,8 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Lambert" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="L-BFGS-B" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Ipopt" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Ipopt" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1199,13 +1198,13 @@
         <v>9178.196769752969</v>
       </c>
       <c r="D2" t="n">
-        <v>9652.607629862499</v>
+        <v>1765.719218805506</v>
       </c>
       <c r="E2" t="n">
-        <v>9777.610855533476</v>
+        <v>2064.473249061879</v>
       </c>
       <c r="F2" t="n">
-        <v>9758.622651391404</v>
+        <v>2181.554976105258</v>
       </c>
     </row>
     <row r="3">
@@ -1219,13 +1218,13 @@
         <v>8873.267468612543</v>
       </c>
       <c r="D3" t="n">
-        <v>9386.37565775182</v>
+        <v>1762.650269182437</v>
       </c>
       <c r="E3" t="n">
-        <v>9524.456728345649</v>
+        <v>2063.548398458318</v>
       </c>
       <c r="F3" t="n">
-        <v>9509.180271300018</v>
+        <v>2181.09215226491</v>
       </c>
     </row>
     <row r="4">
@@ -1242,10 +1241,10 @@
         <v>9115.225827195845</v>
       </c>
       <c r="E4" t="n">
-        <v>9266.917386813388</v>
+        <v>2062.619127233543</v>
       </c>
       <c r="F4" t="n">
-        <v>9255.618547678336</v>
+        <v>2180.627866580358</v>
       </c>
     </row>
     <row r="5">
@@ -1253,7 +1252,7 @@
         <v>40</v>
       </c>
       <c r="B5" t="n">
-        <v>7400.849224747799</v>
+        <v>7400.849210533774</v>
       </c>
       <c r="C5" t="n">
         <v>8246.287654120686</v>
@@ -1262,10 +1261,10 @@
         <v>8839.788780592729</v>
       </c>
       <c r="E5" t="n">
-        <v>9005.437417446605</v>
+        <v>2061.685401564315</v>
       </c>
       <c r="F5" t="n">
-        <v>8998.315579590433</v>
+        <v>2180.162111663959</v>
       </c>
     </row>
     <row r="6">
@@ -1273,7 +1272,7 @@
         <v>50</v>
       </c>
       <c r="B6" t="n">
-        <v>7015.299624452749</v>
+        <v>7015.299610282349</v>
       </c>
       <c r="C6" t="n">
         <v>7926.575170320288</v>
@@ -1285,7 +1284,7 @@
         <v>8740.474739473349</v>
       </c>
       <c r="F6" t="n">
-        <v>8737.660476062158</v>
+        <v>2179.694880076585</v>
       </c>
     </row>
     <row r="7">
@@ -1293,7 +1292,7 @@
         <v>60</v>
       </c>
       <c r="B7" t="n">
-        <v>6628.172212239688</v>
+        <v>6628.172198198248</v>
       </c>
       <c r="C7" t="n">
         <v>7604.316187892881</v>
@@ -1313,10 +1312,10 @@
         <v>70</v>
       </c>
       <c r="B8" t="n">
-        <v>6241.560930093201</v>
+        <v>6241.560916262602</v>
       </c>
       <c r="C8" t="n">
-        <v>7280.720072119769</v>
+        <v>7280.720059276913</v>
       </c>
       <c r="D8" t="n">
         <v>7994.317339934139</v>
@@ -1333,10 +1332,10 @@
         <v>80</v>
       </c>
       <c r="B9" t="n">
-        <v>5857.514714104484</v>
+        <v>5857.51470056202</v>
       </c>
       <c r="C9" t="n">
-        <v>6956.983296776119</v>
+        <v>6956.983283987293</v>
       </c>
       <c r="D9" t="n">
         <v>7708.336047224697</v>
@@ -1353,10 +1352,10 @@
         <v>90</v>
       </c>
       <c r="B10" t="n">
-        <v>5478.004412806918</v>
+        <v>5478.004399624335</v>
       </c>
       <c r="C10" t="n">
-        <v>6634.274231108486</v>
+        <v>6634.27421841964</v>
       </c>
       <c r="D10" t="n">
         <v>7421.39031124111</v>
@@ -1373,10 +1372,10 @@
         <v>100</v>
       </c>
       <c r="B11" t="n">
-        <v>5104.892304656387</v>
+        <v>5104.892291898558</v>
       </c>
       <c r="C11" t="n">
-        <v>6313.719107481405</v>
+        <v>6313.719094936021</v>
       </c>
       <c r="D11" t="n">
         <v>7134.136862116724</v>
@@ -1393,13 +1392,13 @@
         <v>110</v>
       </c>
       <c r="B12" t="n">
-        <v>4739.905197124743</v>
+        <v>4739.90518484865</v>
       </c>
       <c r="C12" t="n">
-        <v>5996.38954065558</v>
+        <v>5996.389528294239</v>
       </c>
       <c r="D12" t="n">
-        <v>6847.21785926257</v>
+        <v>1584.054018959346</v>
       </c>
       <c r="E12" t="n">
         <v>7104.129684136569</v>
@@ -1413,13 +1412,13 @@
         <v>120</v>
       </c>
       <c r="B13" t="n">
-        <v>4384.611972975034</v>
+        <v>4384.61196122973</v>
       </c>
       <c r="C13" t="n">
-        <v>5683.291920475804</v>
+        <v>5683.291908335833</v>
       </c>
       <c r="D13" t="n">
-        <v>6561.257169293547</v>
+        <v>1578.891549717431</v>
       </c>
       <c r="E13" t="n">
         <v>6828.119060707149</v>
@@ -1433,13 +1432,13 @@
         <v>130</v>
       </c>
       <c r="B14" t="n">
-        <v>4040.40627090658</v>
+        <v>4040.406259732463</v>
       </c>
       <c r="C14" t="n">
-        <v>5375.358940665379</v>
+        <v>5375.358928780597</v>
       </c>
       <c r="D14" t="n">
-        <v>6276.857623843</v>
+        <v>1573.659959535943</v>
       </c>
       <c r="E14" t="n">
         <v>6552.440352114487</v>
@@ -1453,13 +1452,13 @@
         <v>140</v>
       </c>
       <c r="B15" t="n">
-        <v>3708.494755196744</v>
+        <v>3708.494744625359</v>
       </c>
       <c r="C15" t="n">
-        <v>5073.443461504155</v>
+        <v>5073.443449904727</v>
       </c>
       <c r="D15" t="n">
-        <v>5994.599412118148</v>
+        <v>1568.357761368935</v>
       </c>
       <c r="E15" t="n">
         <v>6277.564604036372</v>
@@ -1473,16 +1472,16 @@
         <v>150</v>
       </c>
       <c r="B16" t="n">
-        <v>3389.891157764102</v>
+        <v>3389.891147818701</v>
       </c>
       <c r="C16" t="n">
-        <v>4778.314838562854</v>
+        <v>4778.314827275241</v>
       </c>
       <c r="D16" t="n">
-        <v>5715.039771444192</v>
+        <v>1562.983423913132</v>
       </c>
       <c r="E16" t="n">
-        <v>6003.962481002958</v>
+        <v>1904.440097274028</v>
       </c>
       <c r="F16" t="n">
         <v>6036.980004743065</v>
@@ -1493,16 +1492,16 @@
         <v>160</v>
       </c>
       <c r="B17" t="n">
-        <v>3085.415988395215</v>
+        <v>3085.415979090664</v>
       </c>
       <c r="C17" t="n">
-        <v>4490.6577893786</v>
+        <v>4490.657778425652</v>
       </c>
       <c r="D17" t="n">
-        <v>5438.714157017855</v>
+        <v>1557.535369919759</v>
       </c>
       <c r="E17" t="n">
-        <v>5732.107532682902</v>
+        <v>1902.553208482316</v>
       </c>
       <c r="F17" t="n">
         <v>5766.857883661742</v>
@@ -1513,16 +1512,16 @@
         <v>170</v>
       </c>
       <c r="B18" t="n">
-        <v>2795.701530274511</v>
+        <v>2795.701521618217</v>
       </c>
       <c r="C18" t="n">
-        <v>4211.073821537739</v>
+        <v>4211.073810940485</v>
       </c>
       <c r="D18" t="n">
-        <v>5166.139103617379</v>
+        <v>1552.011974427423</v>
       </c>
       <c r="E18" t="n">
-        <v>5462.481116592278</v>
+        <v>2009.661050335671</v>
       </c>
       <c r="F18" t="n">
         <v>5498.526489668206</v>
@@ -1533,19 +1532,19 @@
         <v>180</v>
       </c>
       <c r="B19" t="n">
-        <v>2521.201493156031</v>
+        <v>2521.201485148451</v>
       </c>
       <c r="C19" t="n">
-        <v>3940.085215869218</v>
+        <v>3940.08520564238</v>
       </c>
       <c r="D19" t="n">
-        <v>4897.817041920688</v>
+        <v>1709.108304126345</v>
       </c>
       <c r="E19" t="n">
-        <v>5195.579346662401</v>
+        <v>1959.881648915615</v>
       </c>
       <c r="F19" t="n">
-        <v>5232.494932604319</v>
+        <v>2081.248021815502</v>
       </c>
     </row>
     <row r="20">
@@ -1553,19 +1552,19 @@
         <v>190</v>
       </c>
       <c r="B20" t="n">
-        <v>2262.204505038253</v>
+        <v>2262.204497673873</v>
       </c>
       <c r="C20" t="n">
-        <v>3678.141554127271</v>
+        <v>662.8749848471278</v>
       </c>
       <c r="D20" t="n">
-        <v>4634.243406097018</v>
+        <v>1705.455958898589</v>
       </c>
       <c r="E20" t="n">
-        <v>4931.922542911396</v>
+        <v>1958.374321578865</v>
       </c>
       <c r="F20" t="n">
-        <v>4969.313111828037</v>
+        <v>2080.401177984392</v>
       </c>
     </row>
     <row r="21">
@@ -1573,19 +1572,19 @@
         <v>200</v>
       </c>
       <c r="B21" t="n">
-        <v>2018.850495770847</v>
+        <v>2018.85048903889</v>
       </c>
       <c r="C21" t="n">
-        <v>3425.628808257421</v>
+        <v>635.4061254865912</v>
       </c>
       <c r="D21" t="n">
-        <v>4375.91647395851</v>
+        <v>1701.763879498524</v>
       </c>
       <c r="E21" t="n">
-        <v>4672.067795872001</v>
+        <v>1956.857343022069</v>
       </c>
       <c r="F21" t="n">
-        <v>4709.586730387213</v>
+        <v>2153.715752747054</v>
       </c>
     </row>
     <row r="22">
@@ -1593,19 +1592,19 @@
         <v>210</v>
       </c>
       <c r="B22" t="n">
-        <v>1791.148962272496</v>
+        <v>1791.148956158032</v>
       </c>
       <c r="C22" t="n">
-        <v>3182.881074318052</v>
+        <v>606.9258054122215</v>
       </c>
       <c r="D22" t="n">
-        <v>4123.350522720647</v>
+        <v>1698.031372234107</v>
       </c>
       <c r="E22" t="n">
-        <v>4416.625434452132</v>
+        <v>2004.78417372895</v>
       </c>
       <c r="F22" t="n">
-        <v>4453.996762608031</v>
+        <v>2107.207117671744</v>
       </c>
     </row>
     <row r="23">
@@ -1613,19 +1612,19 @@
         <v>220</v>
       </c>
       <c r="B23" t="n">
-        <v>1578.99809262694</v>
+        <v>1578.998087111802</v>
       </c>
       <c r="C23" t="n">
-        <v>2950.195143739807</v>
+        <v>577.3732502976877</v>
       </c>
       <c r="D23" t="n">
-        <v>3877.093066869811</v>
+        <v>1694.257726684642</v>
       </c>
       <c r="E23" t="n">
-        <v>4166.280396051228</v>
+        <v>2003.547687919376</v>
       </c>
       <c r="F23" t="n">
-        <v>4203.324517213665</v>
+        <v>2106.47298976791</v>
       </c>
     </row>
     <row r="24">
@@ -1633,19 +1632,19 @@
         <v>230</v>
       </c>
       <c r="B24" t="n">
-        <v>1382.203740688203</v>
+        <v>1382.203735751793</v>
       </c>
       <c r="C24" t="n">
-        <v>2727.848260779959</v>
+        <v>546.6825486762696</v>
       </c>
       <c r="D24" t="n">
-        <v>3637.747167340771</v>
+        <v>1690.442215184396</v>
       </c>
       <c r="E24" t="n">
-        <v>3921.819726211555</v>
+        <v>2002.304170117604</v>
       </c>
       <c r="F24" t="n">
-        <v>3958.483648415367</v>
+        <v>2171.023400550012</v>
       </c>
     </row>
     <row r="25">
@@ -1653,19 +1652,19 @@
         <v>240</v>
       </c>
       <c r="B25" t="n">
-        <v>1200.497246535436</v>
+        <v>1200.497242155699</v>
       </c>
       <c r="C25" t="n">
-        <v>2516.119614157306</v>
+        <v>2516.119606375871</v>
       </c>
       <c r="D25" t="n">
-        <v>3406.00004281654</v>
+        <v>1686.584092287006</v>
       </c>
       <c r="E25" t="n">
-        <v>3684.167631562461</v>
+        <v>2001.053556288334</v>
       </c>
       <c r="F25" t="n">
-        <v>3720.56058192499</v>
+        <v>2129.842027406038</v>
       </c>
     </row>
     <row r="26">
@@ -1673,19 +1672,19 @@
         <v>250</v>
       </c>
       <c r="B26" t="n">
-        <v>1033.551037961484</v>
+        <v>1033.55103411552</v>
       </c>
       <c r="C26" t="n">
-        <v>2315.316332755059</v>
+        <v>2315.31632541376</v>
       </c>
       <c r="D26" t="n">
-        <v>3182.659413361101</v>
+        <v>1682.682594209497</v>
       </c>
       <c r="E26" t="n">
-        <v>3454.429553887039</v>
+        <v>1999.795781592889</v>
       </c>
       <c r="F26" t="n">
-        <v>3490.864652635351</v>
+        <v>2129.198432751354</v>
       </c>
     </row>
     <row r="27">
@@ -1693,19 +1692,19 @@
         <v>260</v>
       </c>
       <c r="B27" t="n">
-        <v>880.9907481900703</v>
+        <v>880.9907448547788</v>
       </c>
       <c r="C27" t="n">
-        <v>2125.804941132324</v>
+        <v>2125.804934247563</v>
       </c>
       <c r="D27" t="n">
-        <v>2968.699017200912</v>
+        <v>1678.736938254988</v>
       </c>
       <c r="E27" t="n">
-        <v>3233.946368618893</v>
+        <v>1998.53078037674</v>
       </c>
       <c r="F27" t="n">
-        <v>3270.988418520422</v>
+        <v>2150.351848706534</v>
       </c>
     </row>
     <row r="28">
@@ -1713,19 +1712,19 @@
         <v>270</v>
       </c>
       <c r="B28" t="n">
-        <v>742.4021338565714</v>
+        <v>742.4021310090474</v>
       </c>
       <c r="C28" t="n">
-        <v>1948.049237504124</v>
+        <v>1948.049231096531</v>
       </c>
       <c r="D28" t="n">
-        <v>2765.31425005801</v>
+        <v>1674.746322213266</v>
       </c>
       <c r="E28" t="n">
-        <v>3024.358538932485</v>
+        <v>2038.896830293613</v>
       </c>
       <c r="F28" t="n">
-        <v>3062.876430949377</v>
+        <v>2149.784213615911</v>
       </c>
     </row>
     <row r="29">
@@ -1733,19 +1732,19 @@
         <v>280</v>
       </c>
       <c r="B29" t="n">
-        <v>617.3302114456583</v>
+        <v>617.3302090633276</v>
       </c>
       <c r="C29" t="n">
-        <v>1782.655072365471</v>
+        <v>1782.655066463434</v>
       </c>
       <c r="D29" t="n">
-        <v>2573.987273039629</v>
+        <v>1670.709923738099</v>
       </c>
       <c r="E29" t="n">
-        <v>2827.676994666253</v>
+        <v>2037.845047482746</v>
       </c>
       <c r="F29" t="n">
-        <v>2868.896082166328</v>
+        <v>2149.214552660227</v>
       </c>
     </row>
     <row r="30">
@@ -1753,19 +1752,19 @@
         <v>290</v>
       </c>
       <c r="B30" t="n">
-        <v>505.26652555013</v>
+        <v>505.2665236104544</v>
       </c>
       <c r="C30" t="n">
-        <v>1630.420908369135</v>
+        <v>1630.420903012638</v>
       </c>
       <c r="D30" t="n">
-        <v>2396.557154506394</v>
+        <v>1666.62689970033</v>
       </c>
       <c r="E30" t="n">
-        <v>2646.351304905965</v>
+        <v>2036.787835118314</v>
       </c>
       <c r="F30" t="n">
-        <v>2691.895534237338</v>
+        <v>2691.895527262206</v>
       </c>
     </row>
     <row r="31">
@@ -1773,19 +1772,19 @@
         <v>300</v>
       </c>
       <c r="B31" t="n">
-        <v>405.618078535789</v>
+        <v>405.6180770152896</v>
       </c>
       <c r="C31" t="n">
-        <v>1492.389237711872</v>
+        <v>1492.389232947518</v>
       </c>
       <c r="D31" t="n">
-        <v>2235.283093514282</v>
+        <v>1662.496385515625</v>
       </c>
       <c r="E31" t="n">
-        <v>2483.314848881955</v>
+        <v>2035.725148328328</v>
       </c>
       <c r="F31" t="n">
-        <v>2535.220100394849</v>
+        <v>2167.511305082442</v>
       </c>
     </row>
     <row r="32">
@@ -1793,19 +1792,19 @@
         <v>310</v>
       </c>
       <c r="B32" t="n">
-        <v>317.6481590379963</v>
+        <v>317.648157910221</v>
       </c>
       <c r="C32" t="n">
-        <v>1369.886379055667</v>
+        <v>1369.886374949317</v>
       </c>
       <c r="D32" t="n">
-        <v>2092.876019206588</v>
+        <v>2092.87601382641</v>
       </c>
       <c r="E32" t="n">
-        <v>2341.970869253208</v>
+        <v>2034.656941730144</v>
       </c>
       <c r="F32" t="n">
-        <v>2402.641581352482</v>
+        <v>2167.002889259336</v>
       </c>
     </row>
     <row r="33">
@@ -1813,19 +1812,19 @@
         <v>320</v>
       </c>
       <c r="B33" t="n">
-        <v>240.3759610297583</v>
+        <v>240.3759602617304</v>
       </c>
       <c r="C33" t="n">
-        <v>1264.525758217833</v>
+        <v>1264.525754845939</v>
       </c>
       <c r="D33" t="n">
-        <v>1972.456614429762</v>
+        <v>1972.456610034169</v>
       </c>
       <c r="E33" t="n">
-        <v>2226.067024743022</v>
+        <v>2033.583169422983</v>
       </c>
       <c r="F33" t="n">
-        <v>2298.144202239645</v>
+        <v>2166.492774707582</v>
       </c>
     </row>
     <row r="34">
@@ -1833,19 +1832,19 @@
         <v>330</v>
       </c>
       <c r="B34" t="n">
-        <v>172.4216158293049</v>
+        <v>172.42161537618</v>
       </c>
       <c r="C34" t="n">
-        <v>1178.134887697392</v>
+        <v>1178.134885144083</v>
       </c>
       <c r="D34" t="n">
-        <v>1877.383907668776</v>
+        <v>1877.383904399828</v>
       </c>
       <c r="E34" t="n">
-        <v>2139.40395246876</v>
+        <v>2139.403949546838</v>
       </c>
       <c r="F34" t="n">
-        <v>2225.526476159632</v>
+        <v>2165.98095234534</v>
       </c>
     </row>
     <row r="35">
@@ -1853,19 +1852,19 @@
         <v>340</v>
       </c>
       <c r="B35" t="n">
-        <v>111.7927779814011</v>
+        <v>111.7927777819438</v>
       </c>
       <c r="C35" t="n">
-        <v>1112.560788496384</v>
+        <v>1112.560786841445</v>
       </c>
       <c r="D35" t="n">
-        <v>1810.908316069366</v>
+        <v>1810.908314055027</v>
       </c>
       <c r="E35" t="n">
-        <v>2085.360475019044</v>
+        <v>2085.360473518358</v>
       </c>
       <c r="F35" t="n">
-        <v>2187.844204482997</v>
+        <v>2187.844203687361</v>
       </c>
     </row>
     <row r="36">
@@ -1873,742 +1872,6 @@
         <v>350</v>
       </c>
       <c r="B36" t="n">
-        <v>55.63497493276527</v>
-      </c>
-      <c r="C36" t="n">
-        <v>1069.337205881579</v>
-      </c>
-      <c r="D36" t="n">
-        <v>1775.663524986503</v>
-      </c>
-      <c r="E36" t="n">
-        <v>2066.310425613146</v>
-      </c>
-      <c r="F36" t="n">
-        <v>10243.70442891388</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F36"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="F1" s="1" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B2" t="n">
-        <v>8527.14676018609</v>
-      </c>
-      <c r="C2" t="n">
-        <v>9178.196769752969</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1765.71921880553</v>
-      </c>
-      <c r="E2" t="n">
-        <v>2064.473249061937</v>
-      </c>
-      <c r="F2" t="n">
-        <v>2181.554976105223</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B3" t="n">
-        <v>8158.822563773916</v>
-      </c>
-      <c r="C3" t="n">
-        <v>8873.267468612543</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1762.650269182454</v>
-      </c>
-      <c r="E3" t="n">
-        <v>2063.548398458363</v>
-      </c>
-      <c r="F3" t="n">
-        <v>2181.092152265055</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B4" t="n">
-        <v>7782.716707363538</v>
-      </c>
-      <c r="C4" t="n">
-        <v>8562.247368786357</v>
-      </c>
-      <c r="D4" t="n">
-        <v>9115.225827195845</v>
-      </c>
-      <c r="E4" t="n">
-        <v>2062.619127233601</v>
-      </c>
-      <c r="F4" t="n">
-        <v>2180.627866580501</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="B5" t="n">
-        <v>7400.849210533774</v>
-      </c>
-      <c r="C5" t="n">
-        <v>8246.287654120686</v>
-      </c>
-      <c r="D5" t="n">
-        <v>8839.788780592729</v>
-      </c>
-      <c r="E5" t="n">
-        <v>2061.685401564352</v>
-      </c>
-      <c r="F5" t="n">
-        <v>2180.162111663991</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="B6" t="n">
-        <v>7015.299610282349</v>
-      </c>
-      <c r="C6" t="n">
-        <v>7926.575170320288</v>
-      </c>
-      <c r="D6" t="n">
-        <v>8560.714789200565</v>
-      </c>
-      <c r="E6" t="n">
-        <v>8740.474739473349</v>
-      </c>
-      <c r="F6" t="n">
-        <v>2179.694880076646</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="B7" t="n">
-        <v>6628.172198198248</v>
-      </c>
-      <c r="C7" t="n">
-        <v>7604.316187892881</v>
-      </c>
-      <c r="D7" t="n">
-        <v>8278.667437695844</v>
-      </c>
-      <c r="E7" t="n">
-        <v>8472.497474009471</v>
-      </c>
-      <c r="F7" t="n">
-        <v>8474.051367847143</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>70</v>
-      </c>
-      <c r="B8" t="n">
-        <v>6241.560916262602</v>
-      </c>
-      <c r="C8" t="n">
-        <v>7280.720059276913</v>
-      </c>
-      <c r="D8" t="n">
-        <v>7994.317339934139</v>
-      </c>
-      <c r="E8" t="n">
-        <v>8201.980917192295</v>
-      </c>
-      <c r="F8" t="n">
-        <v>8207.893567243895</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>80</v>
-      </c>
-      <c r="B9" t="n">
-        <v>5857.51470056202</v>
-      </c>
-      <c r="C9" t="n">
-        <v>6956.983283987293</v>
-      </c>
-      <c r="D9" t="n">
-        <v>7708.336047224697</v>
-      </c>
-      <c r="E9" t="n">
-        <v>7929.404712111495</v>
-      </c>
-      <c r="F9" t="n">
-        <v>7939.597954677476</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>90</v>
-      </c>
-      <c r="B10" t="n">
-        <v>5478.004399624335</v>
-      </c>
-      <c r="C10" t="n">
-        <v>6634.27421841964</v>
-      </c>
-      <c r="D10" t="n">
-        <v>7421.39031124111</v>
-      </c>
-      <c r="E10" t="n">
-        <v>7655.25031976745</v>
-      </c>
-      <c r="F10" t="n">
-        <v>7669.579678385311</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="B11" t="n">
-        <v>5104.892291898558</v>
-      </c>
-      <c r="C11" t="n">
-        <v>6313.719094936021</v>
-      </c>
-      <c r="D11" t="n">
-        <v>7134.136862116724</v>
-      </c>
-      <c r="E11" t="n">
-        <v>7379.998895388444</v>
-      </c>
-      <c r="F11" t="n">
-        <v>7398.257262980855</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>110</v>
-      </c>
-      <c r="B12" t="n">
-        <v>4739.90518484865</v>
-      </c>
-      <c r="C12" t="n">
-        <v>5996.389528294239</v>
-      </c>
-      <c r="D12" t="n">
-        <v>1584.054018959368</v>
-      </c>
-      <c r="E12" t="n">
-        <v>7104.129684136569</v>
-      </c>
-      <c r="F12" t="n">
-        <v>7126.052234877594</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>120</v>
-      </c>
-      <c r="B13" t="n">
-        <v>4384.61196122973</v>
-      </c>
-      <c r="C13" t="n">
-        <v>5683.291908335833</v>
-      </c>
-      <c r="D13" t="n">
-        <v>1578.891549717421</v>
-      </c>
-      <c r="E13" t="n">
-        <v>6828.119060707149</v>
-      </c>
-      <c r="F13" t="n">
-        <v>6853.389388809643</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>130</v>
-      </c>
-      <c r="B14" t="n">
-        <v>4040.406259732463</v>
-      </c>
-      <c r="C14" t="n">
-        <v>5375.358928780597</v>
-      </c>
-      <c r="D14" t="n">
-        <v>1573.659959535945</v>
-      </c>
-      <c r="E14" t="n">
-        <v>6552.440352114487</v>
-      </c>
-      <c r="F14" t="n">
-        <v>6580.697841646044</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>140</v>
-      </c>
-      <c r="B15" t="n">
-        <v>3708.494744625359</v>
-      </c>
-      <c r="C15" t="n">
-        <v>5073.443449904727</v>
-      </c>
-      <c r="D15" t="n">
-        <v>1568.35776136894</v>
-      </c>
-      <c r="E15" t="n">
-        <v>6277.564604036372</v>
-      </c>
-      <c r="F15" t="n">
-        <v>6308.413049517874</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>150</v>
-      </c>
-      <c r="B16" t="n">
-        <v>3389.891147818701</v>
-      </c>
-      <c r="C16" t="n">
-        <v>4778.314827275241</v>
-      </c>
-      <c r="D16" t="n">
-        <v>1562.983423913133</v>
-      </c>
-      <c r="E16" t="n">
-        <v>1904.440097274048</v>
-      </c>
-      <c r="F16" t="n">
-        <v>6036.980004743065</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>160</v>
-      </c>
-      <c r="B17" t="n">
-        <v>3085.415979090664</v>
-      </c>
-      <c r="C17" t="n">
-        <v>4490.657778425652</v>
-      </c>
-      <c r="D17" t="n">
-        <v>1557.53536991974</v>
-      </c>
-      <c r="E17" t="n">
-        <v>1902.553208482335</v>
-      </c>
-      <c r="F17" t="n">
-        <v>5766.857883661742</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>170</v>
-      </c>
-      <c r="B18" t="n">
-        <v>2795.701521618217</v>
-      </c>
-      <c r="C18" t="n">
-        <v>4211.073810940485</v>
-      </c>
-      <c r="D18" t="n">
-        <v>1552.011974427415</v>
-      </c>
-      <c r="E18" t="n">
-        <v>2009.661050335726</v>
-      </c>
-      <c r="F18" t="n">
-        <v>5498.526489668206</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>180</v>
-      </c>
-      <c r="B19" t="n">
-        <v>2521.201485148451</v>
-      </c>
-      <c r="C19" t="n">
-        <v>3940.08520564238</v>
-      </c>
-      <c r="D19" t="n">
-        <v>1709.108304126352</v>
-      </c>
-      <c r="E19" t="n">
-        <v>1959.881648915554</v>
-      </c>
-      <c r="F19" t="n">
-        <v>2081.248021815493</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>190</v>
-      </c>
-      <c r="B20" t="n">
-        <v>2262.204497673873</v>
-      </c>
-      <c r="C20" t="n">
-        <v>662.8749848471307</v>
-      </c>
-      <c r="D20" t="n">
-        <v>1705.455958898612</v>
-      </c>
-      <c r="E20" t="n">
-        <v>1958.374321578885</v>
-      </c>
-      <c r="F20" t="n">
-        <v>2080.401177984453</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="B21" t="n">
-        <v>2018.85048903889</v>
-      </c>
-      <c r="C21" t="n">
-        <v>635.4061254865852</v>
-      </c>
-      <c r="D21" t="n">
-        <v>1701.763879498501</v>
-      </c>
-      <c r="E21" t="n">
-        <v>1956.857343022066</v>
-      </c>
-      <c r="F21" t="n">
-        <v>2153.715752747012</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>210</v>
-      </c>
-      <c r="B22" t="n">
-        <v>1791.148956158032</v>
-      </c>
-      <c r="C22" t="n">
-        <v>606.9258054122243</v>
-      </c>
-      <c r="D22" t="n">
-        <v>1698.03137223411</v>
-      </c>
-      <c r="E22" t="n">
-        <v>2004.7841737289</v>
-      </c>
-      <c r="F22" t="n">
-        <v>2107.207117671673</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>220</v>
-      </c>
-      <c r="B23" t="n">
-        <v>1578.998087111802</v>
-      </c>
-      <c r="C23" t="n">
-        <v>577.373250297689</v>
-      </c>
-      <c r="D23" t="n">
-        <v>1694.257726684666</v>
-      </c>
-      <c r="E23" t="n">
-        <v>2003.547687919308</v>
-      </c>
-      <c r="F23" t="n">
-        <v>2106.472989767983</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>230</v>
-      </c>
-      <c r="B24" t="n">
-        <v>1382.203735751793</v>
-      </c>
-      <c r="C24" t="n">
-        <v>546.682548676278</v>
-      </c>
-      <c r="D24" t="n">
-        <v>1690.442215184396</v>
-      </c>
-      <c r="E24" t="n">
-        <v>2002.304170117603</v>
-      </c>
-      <c r="F24" t="n">
-        <v>2171.023400550084</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>240</v>
-      </c>
-      <c r="B25" t="n">
-        <v>1200.497242155699</v>
-      </c>
-      <c r="C25" t="n">
-        <v>2516.119606375871</v>
-      </c>
-      <c r="D25" t="n">
-        <v>1686.584092287009</v>
-      </c>
-      <c r="E25" t="n">
-        <v>2001.053556288294</v>
-      </c>
-      <c r="F25" t="n">
-        <v>2129.842027406107</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>250</v>
-      </c>
-      <c r="B26" t="n">
-        <v>1033.55103411552</v>
-      </c>
-      <c r="C26" t="n">
-        <v>2315.31632541376</v>
-      </c>
-      <c r="D26" t="n">
-        <v>1682.682594209498</v>
-      </c>
-      <c r="E26" t="n">
-        <v>1999.795781592928</v>
-      </c>
-      <c r="F26" t="n">
-        <v>2129.198432751283</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>260</v>
-      </c>
-      <c r="B27" t="n">
-        <v>880.9907448547788</v>
-      </c>
-      <c r="C27" t="n">
-        <v>2125.804934247563</v>
-      </c>
-      <c r="D27" t="n">
-        <v>1678.736938255014</v>
-      </c>
-      <c r="E27" t="n">
-        <v>1998.530780376774</v>
-      </c>
-      <c r="F27" t="n">
-        <v>2150.351848706534</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>270</v>
-      </c>
-      <c r="B28" t="n">
-        <v>742.4021310090474</v>
-      </c>
-      <c r="C28" t="n">
-        <v>1948.049231096531</v>
-      </c>
-      <c r="D28" t="n">
-        <v>1674.746322213278</v>
-      </c>
-      <c r="E28" t="n">
-        <v>2038.896830293613</v>
-      </c>
-      <c r="F28" t="n">
-        <v>2149.784213615911</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>280</v>
-      </c>
-      <c r="B29" t="n">
-        <v>617.3302090633276</v>
-      </c>
-      <c r="C29" t="n">
-        <v>1782.655066463434</v>
-      </c>
-      <c r="D29" t="n">
-        <v>1670.709923738103</v>
-      </c>
-      <c r="E29" t="n">
-        <v>2037.845047482721</v>
-      </c>
-      <c r="F29" t="n">
-        <v>2149.214552660139</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>290</v>
-      </c>
-      <c r="B30" t="n">
-        <v>505.2665236104544</v>
-      </c>
-      <c r="C30" t="n">
-        <v>1630.420903012638</v>
-      </c>
-      <c r="D30" t="n">
-        <v>1666.62689970034</v>
-      </c>
-      <c r="E30" t="n">
-        <v>2036.787835118251</v>
-      </c>
-      <c r="F30" t="n">
-        <v>2691.895527262206</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>300</v>
-      </c>
-      <c r="B31" t="n">
-        <v>405.6180770152896</v>
-      </c>
-      <c r="C31" t="n">
-        <v>1492.389232947518</v>
-      </c>
-      <c r="D31" t="n">
-        <v>1662.496385515611</v>
-      </c>
-      <c r="E31" t="n">
-        <v>2035.725148328296</v>
-      </c>
-      <c r="F31" t="n">
-        <v>2167.511305082347</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>310</v>
-      </c>
-      <c r="B32" t="n">
-        <v>317.648157910221</v>
-      </c>
-      <c r="C32" t="n">
-        <v>1369.886374949317</v>
-      </c>
-      <c r="D32" t="n">
-        <v>2092.87601382641</v>
-      </c>
-      <c r="E32" t="n">
-        <v>2034.656941730121</v>
-      </c>
-      <c r="F32" t="n">
-        <v>2167.002889259323</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>320</v>
-      </c>
-      <c r="B33" t="n">
-        <v>240.3759602617304</v>
-      </c>
-      <c r="C33" t="n">
-        <v>1264.525754845939</v>
-      </c>
-      <c r="D33" t="n">
-        <v>1972.456610034169</v>
-      </c>
-      <c r="E33" t="n">
-        <v>2033.583169422948</v>
-      </c>
-      <c r="F33" t="n">
-        <v>2166.492774707573</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>330</v>
-      </c>
-      <c r="B34" t="n">
-        <v>172.42161537618</v>
-      </c>
-      <c r="C34" t="n">
-        <v>1178.134885144083</v>
-      </c>
-      <c r="D34" t="n">
-        <v>1877.383904399828</v>
-      </c>
-      <c r="E34" t="n">
-        <v>2139.403949546838</v>
-      </c>
-      <c r="F34" t="n">
-        <v>2165.98095234524</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>340</v>
-      </c>
-      <c r="B35" t="n">
-        <v>111.7927777819438</v>
-      </c>
-      <c r="C35" t="n">
-        <v>1112.560786841445</v>
-      </c>
-      <c r="D35" t="n">
-        <v>1810.908314055027</v>
-      </c>
-      <c r="E35" t="n">
-        <v>2085.360473518358</v>
-      </c>
-      <c r="F35" t="n">
-        <v>2187.844203687361</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>350</v>
-      </c>
-      <c r="B36" t="n">
         <v>55.63497489163242</v>
       </c>
       <c r="C36" t="n">
@@ -2621,7 +1884,7 @@
         <v>2066.310425604778</v>
       </c>
       <c r="F36" t="n">
-        <v>2182.476267549292</v>
+        <v>2182.476267549295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>